<commit_message>
Finalisation des uses cases et scénarios
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\TPI\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/TPI/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1FBC5B90-C450-1B44-82BE-FBADA61053EA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="28800" windowHeight="16485"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Commencement du TPI. J'ai reçu mon cahier des charges que j'ai signé. J'ai eu un entretien avec l'expert 1.</t>
   </si>
@@ -41,13 +42,13 @@
     <t>Création des maquettes pour le site.</t>
   </si>
   <si>
-    <t>3 heures</t>
+    <t xml:space="preserve">Création des uses cases et scénarios </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -359,19 +360,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="96.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="96.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>43228</v>
       </c>
@@ -382,7 +383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43228</v>
       </c>
@@ -393,7 +394,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43228</v>
       </c>
@@ -401,7 +402,18 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>43228</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout de choses dans la doc et de l'activité d'aujourd'hui dans le journal de travail
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/TPI/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\TPI\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1FBC5B90-C450-1B44-82BE-FBADA61053EA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="28800" windowHeight="16485"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Commencement du TPI. J'ai reçu mon cahier des charges que j'ai signé. J'ai eu un entretien avec l'expert 1.</t>
   </si>
@@ -43,12 +42,18 @@
   </si>
   <si>
     <t xml:space="preserve">Création des uses cases et scénarios </t>
+  </si>
+  <si>
+    <t>Commencer à faire le MCD et le MLD. Je les ai montrés à M. Chavey et on en a parlé puis amené quelques modifications.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 heures </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -360,19 +365,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="96.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="109.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>43228</v>
       </c>
@@ -383,7 +388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43228</v>
       </c>
@@ -394,7 +399,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43228</v>
       </c>
@@ -405,7 +410,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43228</v>
       </c>
@@ -414,6 +419,17 @@
       </c>
       <c r="C4" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43229</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modification du temps pour une activité
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\TPI\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/TPI/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{106A0AC7-0311-F044-8956-95538AF6AFAD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="28800" windowHeight="16485"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -47,13 +48,13 @@
     <t>Commencer à faire le MCD et le MLD. Je les ai montrés à M. Chavey et on en a parlé puis amené quelques modifications.</t>
   </si>
   <si>
-    <t xml:space="preserve">4 heures </t>
+    <t xml:space="preserve">5 heures </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -365,19 +366,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="109.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="109.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>43228</v>
       </c>
@@ -388,7 +389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43228</v>
       </c>
@@ -399,7 +400,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43228</v>
       </c>
@@ -410,7 +411,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43228</v>
       </c>
@@ -421,7 +422,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43229</v>
       </c>

</xml_diff>

<commit_message>
Ajout d'un pdf et des tâches effectuées
J'ai tout rajouté dans le journal de travail
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/TPI/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\TPI\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{106A0AC7-0311-F044-8956-95538AF6AFAD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="28800" windowHeight="16485"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Commencement du TPI. J'ai reçu mon cahier des charges que j'ai signé. J'ai eu un entretien avec l'expert 1.</t>
   </si>
@@ -48,13 +47,22 @@
     <t>Commencer à faire le MCD et le MLD. Je les ai montrés à M. Chavey et on en a parlé puis amené quelques modifications.</t>
   </si>
   <si>
-    <t xml:space="preserve">5 heures </t>
+    <t>Finalisation du MLD/MCD.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.5 heures </t>
+  </si>
+  <si>
+    <t>0.5 heure</t>
+  </si>
+  <si>
+    <t>Commencement de la documentation du projet. Rédiger l'introduction, les objectifs et la planification initiale.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -366,19 +374,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="109.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="109.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>43228</v>
       </c>
@@ -389,7 +397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43228</v>
       </c>
@@ -400,7 +408,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43228</v>
       </c>
@@ -411,7 +419,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43228</v>
       </c>
@@ -422,7 +430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43229</v>
       </c>
@@ -430,11 +438,33 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>43229</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>43235</v>
+      </c>
+      <c r="B7" t="s">
         <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="152" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="152" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Petit changement dans le fichier
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\TPI\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/TPI/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E8FB2721-F818-DF44-9815-6E8A92259BAD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="28800" windowHeight="16485"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -384,19 +385,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="109.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="109.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>43228</v>
       </c>
@@ -407,7 +408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43228</v>
       </c>
@@ -418,7 +419,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43228</v>
       </c>
@@ -429,7 +430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43228</v>
       </c>
@@ -440,7 +441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43229</v>
       </c>
@@ -451,7 +452,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43229</v>
       </c>
@@ -462,7 +463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43235</v>
       </c>
@@ -473,7 +474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43235</v>
       </c>

</xml_diff>

<commit_message>
Ajout de la tâche de la journée
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Commencement du TPI. J'ai reçu mon cahier des charges que j'ai signé. J'ai eu un entretien avec l'expert 1.</t>
   </si>
@@ -71,9 +71,6 @@
     <t>J'ai commencé à envoyer des requête à ma base de données depuis mon application mobile, en me référant à une vidéo trouvée sur youtube mais j'ai eu des soucis. Du coup je n'arrivais pas à envoyer ma requête.</t>
   </si>
   <si>
-    <t>https://www.youtube.com/watch?v=1v-BbgFM5ps</t>
-  </si>
-  <si>
     <t>Suite à mon problème, M. Chavey est venu me donner un coup de main afin de débuguer pour que je puisse continuer à travailler mais nous n'avons pas trouvé la solution.</t>
   </si>
   <si>
@@ -83,7 +80,10 @@
     <t>3 heures</t>
   </si>
   <si>
-    <t xml:space="preserve">Une des deux pages de mon application mobile est terminée, j'ai commencé à faire la deuxième page. Je peux déjà ajouté un mouvement quand j'ajoute des bouteilles dans ma cave. Elle reprend les ID de la bouteille et de l'utilisateur qui l'a ajouté </t>
+    <t>Une des deux pages de mon application mobile est terminée, j'ai commencé à faire la deuxième page. Je peux déjà ajouter un mouvement quand j'ajoute des bouteilles dans ma cave. Elle reprend aussi le fait qu'une personne enlève une bouteille et cela crée un mouvement dans la BD.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai fait de la documentation, j'ai ajouté mes maquettes et aimélioré des uses cases et scénarios </t>
   </si>
 </sst>
 </file>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,7 +416,7 @@
     <col min="2" max="2" width="112.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>43228</v>
       </c>
@@ -427,7 +427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43228</v>
       </c>
@@ -438,7 +438,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43228</v>
       </c>
@@ -449,7 +449,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43228</v>
       </c>
@@ -460,7 +460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43229</v>
       </c>
@@ -471,7 +471,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43229</v>
       </c>
@@ -482,7 +482,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43235</v>
       </c>
@@ -493,7 +493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43235</v>
       </c>
@@ -504,7 +504,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43236</v>
       </c>
@@ -515,40 +515,48 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43236</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43237</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43237</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>43237</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C12" t="s">
-        <v>18</v>
+      <c r="C13" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>